<commit_message>
Magnetic sensor library update
Added direct download link to the magnetic sensor library and added instructions on how to import it into Arduino
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Willow_Joystick_BOM.xlsx
+++ b/Documentation/Working_Documents/Willow_Joystick_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 24-12 Willow Joystick/Willow-Joystick/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc-my.sharepoint.com/personal/bradw_neilsquire_ca/Documents/Documents/GitHub/Willow-Joystick/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="794" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F636EE4-A56C-4CE1-8B85-01A9D1E43D6A}"/>
+  <xr:revisionPtr revIDLastSave="813" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B200AA3A-67B7-4646-8B17-D3E7C16E5312}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -551,9 +551,6 @@
     <t>PAN HEAD SCREW_M3 X 8MM CROSS SL</t>
   </si>
   <si>
-    <t>97790803111 Würth Elektronik | Hardware, Fasteners, Accessories | DigiKey</t>
-  </si>
-  <si>
     <t>Bumper Specialties Inc.</t>
   </si>
   <si>
@@ -645,6 +642,9 @@
   </si>
   <si>
     <t>Joystick topper that is compatible with mouldable plastic pellets</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/w%C3%BCrth-elektronik/97790803111/10056388?s=N4IgTCBcDaIJwHYFwAwA4UGYCMuQF0BfIA</t>
   </si>
 </sst>
 </file>
@@ -1162,6 +1162,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="14" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="14" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="10" borderId="20" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="11" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1183,13 +1190,6 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="19" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="9" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="5" fillId="10" borderId="20" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="11" xfId="4" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1490,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EE8AD1-7DB5-46E4-9BCF-A08DFBDA7B00}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,24 +1516,24 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1543,15 +1543,15 @@
       <c r="B3" s="62">
         <v>45723</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I4" s="75" t="s">
+      <c r="I4" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="76"/>
-      <c r="K4" s="72" t="s">
+      <c r="J4" s="69"/>
+      <c r="K4" s="65" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="53" t="s">
@@ -1566,12 +1566,12 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="I5" s="77">
+      <c r="I5" s="70">
         <f>SUM(H42:H66)</f>
         <v>169</v>
       </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="73">
+      <c r="J5" s="71"/>
+      <c r="K5" s="66">
         <f>K6+K67+K40</f>
         <v>135.23620000000003</v>
       </c>
@@ -1645,22 +1645,22 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="68"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="75"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
@@ -1975,7 +1975,7 @@
         <v>101</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>111</v>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="M17" s="16"/>
       <c r="N17" s="64" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -2060,7 +2060,7 @@
         <v>101</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>111</v>
@@ -2092,22 +2092,22 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="71"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="78"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
@@ -3039,7 +3039,7 @@
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="23"/>
       <c r="B42" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>143</v>
@@ -3078,7 +3078,7 @@
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>144</v>
@@ -3117,7 +3117,7 @@
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>145</v>
@@ -3156,7 +3156,7 @@
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>145</v>
@@ -3195,7 +3195,7 @@
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>146</v>
@@ -3234,7 +3234,7 @@
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>147</v>
@@ -3273,7 +3273,7 @@
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>148</v>
@@ -3312,7 +3312,7 @@
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>149</v>
@@ -3351,7 +3351,7 @@
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>149</v>
@@ -3390,7 +3390,7 @@
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>150</v>
@@ -3429,7 +3429,7 @@
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>151</v>
@@ -3468,7 +3468,7 @@
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="18"/>
       <c r="B53" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>152</v>
@@ -3507,10 +3507,10 @@
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="18"/>
       <c r="B54" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C54" s="18" t="s">
         <v>201</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>202</v>
       </c>
       <c r="D54" s="23" t="s">
         <v>20</v>
@@ -3546,7 +3546,7 @@
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
       <c r="B55" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>153</v>
@@ -3585,7 +3585,7 @@
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="18"/>
       <c r="B56" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>154</v>
@@ -3624,7 +3624,7 @@
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
       <c r="B57" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>155</v>
@@ -3663,7 +3663,7 @@
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="18"/>
       <c r="B58" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>156</v>
@@ -3702,7 +3702,7 @@
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="18"/>
       <c r="B59" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>157</v>
@@ -3741,7 +3741,7 @@
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="18"/>
       <c r="B60" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>158</v>
@@ -3780,7 +3780,7 @@
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="18"/>
       <c r="B61" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>159</v>
@@ -3819,7 +3819,7 @@
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="18"/>
       <c r="B62" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C62" s="18" t="s">
         <v>160</v>
@@ -3858,10 +3858,10 @@
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="18"/>
       <c r="B63" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D63" s="23" t="s">
         <v>20</v>
@@ -3897,10 +3897,10 @@
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="18"/>
       <c r="B64" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" s="18" t="s">
         <v>195</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>196</v>
       </c>
       <c r="D64" s="23" t="s">
         <v>20</v>
@@ -3936,7 +3936,7 @@
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="18"/>
       <c r="B65" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>161</v>
@@ -3975,7 +3975,7 @@
     <row r="66" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
       <c r="B66" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>162</v>
@@ -4579,9 +4579,10 @@
     <hyperlink ref="N15" r:id="rId27" xr:uid="{17A87E0D-D8AD-46C4-9CB4-C2C3AEA4AE8B}"/>
     <hyperlink ref="N18" r:id="rId28" xr:uid="{941B0276-FED2-4609-954C-259FDB9F3A1A}"/>
     <hyperlink ref="N16" r:id="rId29" xr:uid="{331D2496-D6A7-4884-9C01-2C7D0AD11696}"/>
+    <hyperlink ref="N17" r:id="rId30" xr:uid="{3BE7BE7D-2203-4102-9BA3-E67D9E7D2E96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -4595,17 +4596,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1619f065ca3ee2b2a551d697af78a52c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f162289ff582f7dcdaca5148f0118a53" ns2:_="" ns3:_="">
     <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
@@ -4860,6 +4850,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
@@ -4869,6 +4870,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AADA0EB-AE5F-4308-A18F-9BF4422BC6F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4877,8 +4897,4 @@
     <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AADA0EB-AE5F-4308-A18F-9BF4422BC6F9}"/>
 </file>
</xml_diff>